<commit_message>
correctly exporting file to excel, and recover of leaves by admin
</commit_message>
<xml_diff>
--- a/excel_database.xlsx
+++ b/excel_database.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Registrados" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dane" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Urlopy" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,11 +461,6 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>password</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>days_left</t>
         </is>
       </c>
@@ -487,12 +487,7 @@
           <t>Admin</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>$2b$12$bOho4HXCPlHIfdkmFKwPoerkqYANlAk0kqZ8up31qGW5s/EEjDuRm</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2" t="n">
         <v>26</v>
       </c>
     </row>
@@ -518,13 +513,184 @@
           <t>user</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>$2b$12$fReVqCeJryx6uWtEhRjFseAA7oU.XK5iYqBheb6/agG08g2PcvvFy</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>16</v>
+      <c r="F3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>start_day</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>end_day</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>deleted</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>44715</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44720</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>test123</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>44724</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>44728</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>test123</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>44737</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44737</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>test123</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>44734</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44734</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>test123</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44738</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>44749</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>